<commit_message>
report kertas kerja v2
</commit_message>
<xml_diff>
--- a/report/template/PEROLEHAN/revisi-template_kk_v3.xlsx
+++ b/report/template/PEROLEHAN/revisi-template_kk_v3.xlsx
@@ -86,10 +86,11 @@
     <t xml:space="preserve">SALDO AKHIR</t>
   </si>
   <si>
-    <t xml:space="preserve">KET</t>
+    <t xml:space="preserve">Riwayat</t>
   </si>
   <si>
-    <t xml:space="preserve">KOREKSI TAMBAH TERHADAP SALDO AWAL [kk.tahun]</t>
+    <t xml:space="preserve">Koreksi Tambah Terhadap Saldo Awal 
+[kk.tahun]</t>
   </si>
   <si>
     <t xml:space="preserve">REALISASI BELANJA MODAL</t>
@@ -150,19 +151,16 @@
     <t xml:space="preserve">Nilai Buku</t>
   </si>
   <si>
-    <t xml:space="preserve">ASET BARU</t>
+    <t xml:space="preserve">Aset Baru</t>
   </si>
   <si>
-    <t xml:space="preserve">KAPITALISASI</t>
+    <t xml:space="preserve">Kapitalisasi</t>
   </si>
   <si>
-    <t xml:space="preserve">JUMLAH DARI BM</t>
+    <t xml:space="preserve">Jumlah Dari BM</t>
   </si>
   <si>
-    <t xml:space="preserve">Aset BARU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL</t>
+    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">DIHIBAHKAN</t>
@@ -258,6 +256,9 @@
   </si>
   <si>
     <t xml:space="preserve">[a.bj_total_brg;block=tbs:row;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[a.bj_total_nilai;block=tbs:row;ope=tbs:num]</t>
   </si>
   <si>
     <t xml:space="preserve">[a.hibah_jml;block=tbs:row;ope=tbs:num]</t>
@@ -445,14 +446,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FF93CDDD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF93CDDD"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -579,7 +580,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="95">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -588,107 +589,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -716,10 +621,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -732,11 +633,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,11 +645,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -772,7 +669,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -800,7 +697,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -816,7 +713,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -864,7 +761,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,7 +785,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -908,7 +805,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -964,7 +861,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -972,11 +873,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1016,11 +913,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1054,6 +951,10 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1143,9 +1044,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>167760</xdr:colOff>
+      <xdr:colOff>166320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1159,7 +1060,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="133560" y="0"/>
-          <a:ext cx="529200" cy="719640"/>
+          <a:ext cx="527760" cy="718200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1181,126 +1082,78 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AY4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BF19" activeCellId="0" sqref="BF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="1" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.8010204081633"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="8" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="10" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="11" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="12" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="13" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="15" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="16" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="17" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="18" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="19" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="9" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="9" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="20" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="21" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="38" min="37" style="22" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="23" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="24" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="25" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="26" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="26" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="26" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="26" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="27" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="26" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="20" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="21" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="52" min="51" style="21" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="8" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="8" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="9" width="13.5"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="9" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="9" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="58" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="6.75"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="3" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="3" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="3" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="3" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="38" min="37" style="3" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="2" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="3" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="3" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="3" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="3" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="3" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="3" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="3" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="3" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="52" min="51" style="3" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="2" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="2" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="3" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="3" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="3" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="1" width="52.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="59" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="0"/>
-      <c r="C1" s="28"/>
+      <c r="C1" s="4"/>
       <c r="D1" s="0"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="0"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="30"/>
+      <c r="L1" s="6"/>
       <c r="M1" s="0"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
-      <c r="AU1" s="4"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="4"/>
-      <c r="AX1" s="5"/>
-      <c r="AY1" s="5"/>
-      <c r="AZ1" s="5"/>
-      <c r="BA1" s="5"/>
-      <c r="BB1" s="4"/>
-      <c r="BC1" s="5"/>
-      <c r="BD1" s="5"/>
-      <c r="BE1" s="5"/>
+      <c r="BA1" s="3"/>
       <c r="BF1" s="0"/>
       <c r="BG1" s="0"/>
       <c r="BH1" s="0"/>
@@ -2272,63 +2125,16 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="0"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="30"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="0"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="4"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
+      <c r="BA2" s="3"/>
       <c r="BF2" s="0"/>
       <c r="BG2" s="0"/>
       <c r="BH2" s="0"/>
@@ -3301,62 +3107,15 @@
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
       <c r="C3" s="0"/>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="0"/>
-      <c r="F3" s="29"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="0"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="30"/>
+      <c r="L3" s="6"/>
       <c r="M3" s="0"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="5"/>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="5"/>
-      <c r="AQ3" s="5"/>
-      <c r="AR3" s="5"/>
-      <c r="AS3" s="5"/>
-      <c r="AT3" s="5"/>
-      <c r="AU3" s="4"/>
-      <c r="AV3" s="5"/>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="5"/>
-      <c r="AY3" s="5"/>
-      <c r="AZ3" s="5"/>
-      <c r="BA3" s="5"/>
-      <c r="BB3" s="4"/>
-      <c r="BC3" s="5"/>
-      <c r="BD3" s="5"/>
-      <c r="BE3" s="5"/>
+      <c r="BA3" s="3"/>
       <c r="BF3" s="0"/>
       <c r="BG3" s="0"/>
       <c r="BH3" s="0"/>
@@ -4331,58 +4090,11 @@
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
-      <c r="F4" s="29"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="0"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="30"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="0"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="5"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="5"/>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="5"/>
-      <c r="AS4" s="5"/>
-      <c r="AT4" s="5"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="5"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="5"/>
-      <c r="AY4" s="5"/>
-      <c r="AZ4" s="5"/>
-      <c r="BA4" s="5"/>
-      <c r="BB4" s="4"/>
-      <c r="BC4" s="5"/>
-      <c r="BD4" s="5"/>
-      <c r="BE4" s="5"/>
+      <c r="BA4" s="3"/>
       <c r="BF4" s="0"/>
       <c r="BG4" s="0"/>
       <c r="BH4" s="0"/>
@@ -5357,58 +5069,11 @@
       <c r="C5" s="0"/>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
-      <c r="F5" s="29"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="0"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="30"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="0"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="5"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="5"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
-      <c r="AT5" s="5"/>
-      <c r="AU5" s="4"/>
-      <c r="AV5" s="5"/>
-      <c r="AW5" s="4"/>
-      <c r="AX5" s="5"/>
-      <c r="AY5" s="5"/>
-      <c r="AZ5" s="5"/>
-      <c r="BA5" s="5"/>
-      <c r="BB5" s="4"/>
-      <c r="BC5" s="5"/>
-      <c r="BD5" s="5"/>
-      <c r="BE5" s="5"/>
+      <c r="BA5" s="3"/>
       <c r="BF5" s="0"/>
       <c r="BG5" s="0"/>
       <c r="BH5" s="0"/>
@@ -6378,67 +6043,21 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="0"/>
+      <c r="G6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="30"/>
+      <c r="H6" s="0"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="0"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="5"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="5"/>
-      <c r="AQ6" s="5"/>
-      <c r="AR6" s="5"/>
-      <c r="AS6" s="5"/>
-      <c r="AT6" s="5"/>
-      <c r="AU6" s="4"/>
-      <c r="AV6" s="5"/>
-      <c r="AW6" s="4"/>
-      <c r="AX6" s="5"/>
-      <c r="AY6" s="5"/>
-      <c r="AZ6" s="5"/>
-      <c r="BA6" s="5"/>
-      <c r="BB6" s="4"/>
-      <c r="BC6" s="5"/>
-      <c r="BD6" s="5"/>
-      <c r="BE6" s="5"/>
+      <c r="BA6" s="3"/>
       <c r="BF6" s="0"/>
       <c r="BG6" s="0"/>
       <c r="BH6" s="0"/>
@@ -7408,67 +7027,21 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="0"/>
+      <c r="G7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="30"/>
+      <c r="H7" s="0"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="0"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5"/>
-      <c r="AG7" s="5"/>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="5"/>
-      <c r="AJ7" s="5"/>
-      <c r="AK7" s="5"/>
-      <c r="AL7" s="5"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="5"/>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="5"/>
-      <c r="AQ7" s="5"/>
-      <c r="AR7" s="5"/>
-      <c r="AS7" s="5"/>
-      <c r="AT7" s="5"/>
-      <c r="AU7" s="4"/>
-      <c r="AV7" s="5"/>
-      <c r="AW7" s="4"/>
-      <c r="AX7" s="5"/>
-      <c r="AY7" s="5"/>
-      <c r="AZ7" s="5"/>
-      <c r="BA7" s="5"/>
-      <c r="BB7" s="4"/>
-      <c r="BC7" s="5"/>
-      <c r="BD7" s="5"/>
-      <c r="BE7" s="5"/>
+      <c r="BA7" s="3"/>
       <c r="BF7" s="0"/>
       <c r="BG7" s="0"/>
       <c r="BH7" s="0"/>
@@ -8438,67 +8011,21 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="0"/>
+      <c r="G8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="30"/>
+      <c r="H8" s="0"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="0"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="5"/>
-      <c r="AO8" s="4"/>
-      <c r="AP8" s="5"/>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="5"/>
-      <c r="AS8" s="5"/>
-      <c r="AT8" s="5"/>
-      <c r="AU8" s="4"/>
-      <c r="AV8" s="5"/>
-      <c r="AW8" s="4"/>
-      <c r="AX8" s="5"/>
-      <c r="AY8" s="5"/>
-      <c r="AZ8" s="5"/>
-      <c r="BA8" s="5"/>
-      <c r="BB8" s="4"/>
-      <c r="BC8" s="5"/>
-      <c r="BD8" s="5"/>
-      <c r="BE8" s="5"/>
+      <c r="BA8" s="3"/>
       <c r="BF8" s="0"/>
       <c r="BG8" s="0"/>
       <c r="BH8" s="0"/>
@@ -9468,67 +8995,21 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="33" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="30"/>
+      <c r="H9" s="0"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="0"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="5"/>
-      <c r="AO9" s="4"/>
-      <c r="AP9" s="5"/>
-      <c r="AQ9" s="5"/>
-      <c r="AR9" s="5"/>
-      <c r="AS9" s="5"/>
-      <c r="AT9" s="5"/>
-      <c r="AU9" s="4"/>
-      <c r="AV9" s="5"/>
-      <c r="AW9" s="4"/>
-      <c r="AX9" s="5"/>
-      <c r="AY9" s="5"/>
-      <c r="AZ9" s="5"/>
-      <c r="BA9" s="5"/>
-      <c r="BB9" s="4"/>
-      <c r="BC9" s="5"/>
-      <c r="BD9" s="5"/>
-      <c r="BE9" s="5"/>
+      <c r="BA9" s="3"/>
       <c r="BF9" s="0"/>
       <c r="BG9" s="0"/>
       <c r="BH9" s="0"/>
@@ -10498,67 +9979,21 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="33" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="30"/>
+      <c r="H10" s="0"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="0"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="4"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="4"/>
-      <c r="AP10" s="5"/>
-      <c r="AQ10" s="5"/>
-      <c r="AR10" s="5"/>
-      <c r="AS10" s="5"/>
-      <c r="AT10" s="5"/>
-      <c r="AU10" s="4"/>
-      <c r="AV10" s="5"/>
-      <c r="AW10" s="4"/>
-      <c r="AX10" s="5"/>
-      <c r="AY10" s="5"/>
-      <c r="AZ10" s="5"/>
-      <c r="BA10" s="5"/>
-      <c r="BB10" s="4"/>
-      <c r="BC10" s="5"/>
-      <c r="BD10" s="5"/>
-      <c r="BE10" s="5"/>
+      <c r="BA10" s="3"/>
       <c r="BF10" s="0"/>
       <c r="BG10" s="0"/>
       <c r="BH10" s="0"/>
@@ -11528,67 +10963,21 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="0"/>
+      <c r="G11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="30"/>
+      <c r="H11" s="0"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="0"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="4"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="4"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="5"/>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="5"/>
-      <c r="AJ11" s="5"/>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="5"/>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="5"/>
-      <c r="AO11" s="4"/>
-      <c r="AP11" s="5"/>
-      <c r="AQ11" s="5"/>
-      <c r="AR11" s="5"/>
-      <c r="AS11" s="5"/>
-      <c r="AT11" s="5"/>
-      <c r="AU11" s="4"/>
-      <c r="AV11" s="5"/>
-      <c r="AW11" s="4"/>
-      <c r="AX11" s="5"/>
-      <c r="AY11" s="5"/>
-      <c r="AZ11" s="5"/>
-      <c r="BA11" s="5"/>
-      <c r="BB11" s="4"/>
-      <c r="BC11" s="5"/>
-      <c r="BD11" s="5"/>
-      <c r="BE11" s="5"/>
+      <c r="BA11" s="3"/>
       <c r="BF11" s="0"/>
       <c r="BG11" s="0"/>
       <c r="BH11" s="0"/>
@@ -12565,56 +11954,9 @@
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="30"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="0"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="5"/>
-      <c r="AJ12" s="5"/>
-      <c r="AK12" s="5"/>
-      <c r="AL12" s="5"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="5"/>
-      <c r="AO12" s="4"/>
-      <c r="AP12" s="5"/>
-      <c r="AQ12" s="5"/>
-      <c r="AR12" s="5"/>
-      <c r="AS12" s="5"/>
-      <c r="AT12" s="5"/>
-      <c r="AU12" s="4"/>
-      <c r="AV12" s="5"/>
-      <c r="AW12" s="4"/>
-      <c r="AX12" s="5"/>
-      <c r="AY12" s="5"/>
-      <c r="AZ12" s="5"/>
-      <c r="BA12" s="5"/>
-      <c r="BB12" s="4"/>
-      <c r="BC12" s="5"/>
-      <c r="BD12" s="5"/>
-      <c r="BE12" s="5"/>
+      <c r="BA12" s="3"/>
       <c r="BF12" s="0"/>
       <c r="BG12" s="0"/>
       <c r="BH12" s="0"/>
@@ -13583,175 +12925,175 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" s="40" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
+    <row r="13" s="15" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37" t="s">
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="37"/>
-      <c r="X13" s="37"/>
-      <c r="Y13" s="37"/>
-      <c r="Z13" s="37"/>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37"/>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37"/>
-      <c r="AE13" s="37"/>
-      <c r="AF13" s="37"/>
-      <c r="AG13" s="37"/>
-      <c r="AH13" s="37" t="s">
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="12"/>
+      <c r="AH13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AI13" s="37"/>
-      <c r="AJ13" s="37"/>
-      <c r="AK13" s="37"/>
-      <c r="AL13" s="37"/>
-      <c r="AM13" s="37"/>
-      <c r="AN13" s="37"/>
-      <c r="AO13" s="37"/>
-      <c r="AP13" s="37"/>
-      <c r="AQ13" s="37"/>
-      <c r="AR13" s="37"/>
-      <c r="AS13" s="37"/>
-      <c r="AT13" s="37"/>
-      <c r="AU13" s="37"/>
-      <c r="AV13" s="37"/>
-      <c r="AW13" s="37"/>
-      <c r="AX13" s="37"/>
-      <c r="AY13" s="37"/>
-      <c r="AZ13" s="37"/>
-      <c r="BA13" s="38" t="s">
+      <c r="AI13" s="12"/>
+      <c r="AJ13" s="12"/>
+      <c r="AK13" s="12"/>
+      <c r="AL13" s="12"/>
+      <c r="AM13" s="12"/>
+      <c r="AN13" s="12"/>
+      <c r="AO13" s="12"/>
+      <c r="AP13" s="12"/>
+      <c r="AQ13" s="12"/>
+      <c r="AR13" s="12"/>
+      <c r="AS13" s="12"/>
+      <c r="AT13" s="12"/>
+      <c r="AU13" s="12"/>
+      <c r="AV13" s="12"/>
+      <c r="AW13" s="12"/>
+      <c r="AX13" s="12"/>
+      <c r="AY13" s="12"/>
+      <c r="AZ13" s="12"/>
+      <c r="BA13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="BB13" s="38"/>
-      <c r="BC13" s="38"/>
-      <c r="BD13" s="38"/>
-      <c r="BE13" s="38"/>
-      <c r="BF13" s="39" t="s">
+      <c r="BB13" s="13"/>
+      <c r="BC13" s="13"/>
+      <c r="BD13" s="13"/>
+      <c r="BE13" s="13"/>
+      <c r="BF13" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="41" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42" t="s">
+      <c r="M14" s="14"/>
+      <c r="N14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="38" t="s">
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="38"/>
-      <c r="V14" s="43" t="s">
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="W14" s="43"/>
-      <c r="X14" s="44" t="s">
+      <c r="W14" s="17"/>
+      <c r="X14" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="Y14" s="44"/>
-      <c r="Z14" s="45" t="s">
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AA14" s="45"/>
-      <c r="AB14" s="46" t="s">
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="47" t="s">
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="48" t="s">
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AG14" s="48" t="s">
+      <c r="AG14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AH14" s="49" t="s">
+      <c r="AH14" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AI14" s="49"/>
-      <c r="AJ14" s="50" t="s">
+      <c r="AI14" s="23"/>
+      <c r="AJ14" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AK14" s="50"/>
-      <c r="AL14" s="50"/>
-      <c r="AM14" s="50"/>
-      <c r="AN14" s="50"/>
-      <c r="AO14" s="51" t="s">
+      <c r="AK14" s="24"/>
+      <c r="AL14" s="24"/>
+      <c r="AM14" s="24"/>
+      <c r="AN14" s="24"/>
+      <c r="AO14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="AP14" s="51"/>
-      <c r="AQ14" s="52" t="s">
+      <c r="AP14" s="25"/>
+      <c r="AQ14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AR14" s="52"/>
-      <c r="AS14" s="52"/>
-      <c r="AT14" s="52"/>
-      <c r="AU14" s="52"/>
-      <c r="AV14" s="52"/>
-      <c r="AW14" s="49" t="s">
+      <c r="AR14" s="26"/>
+      <c r="AS14" s="26"/>
+      <c r="AT14" s="26"/>
+      <c r="AU14" s="26"/>
+      <c r="AV14" s="26"/>
+      <c r="AW14" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AX14" s="49"/>
-      <c r="AY14" s="53" t="s">
+      <c r="AX14" s="23"/>
+      <c r="AY14" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AZ14" s="53" t="s">
+      <c r="AZ14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="BA14" s="38"/>
-      <c r="BB14" s="38"/>
-      <c r="BC14" s="38"/>
-      <c r="BD14" s="38"/>
-      <c r="BE14" s="38"/>
-      <c r="BF14" s="39"/>
+      <c r="BA14" s="13"/>
+      <c r="BB14" s="13"/>
+      <c r="BC14" s="13"/>
+      <c r="BD14" s="13"/>
+      <c r="BE14" s="13"/>
+      <c r="BF14" s="14"/>
       <c r="BG14" s="0"/>
       <c r="BH14" s="0"/>
       <c r="BI14" s="0"/>
@@ -14720,108 +14062,108 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="54" t="s">
+      <c r="I15" s="11"/>
+      <c r="J15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42" t="s">
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="42" t="s">
+      <c r="O15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="P15" s="55" t="s">
+      <c r="P15" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="38" t="s">
+      <c r="Q15" s="29"/>
+      <c r="R15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="S15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T15" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S15" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="T15" s="38" t="s">
+      <c r="U15" s="13"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="21"/>
+      <c r="AE15" s="21"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
+      <c r="AH15" s="23"/>
+      <c r="AI15" s="23"/>
+      <c r="AJ15" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="U15" s="38"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="43"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="44"/>
-      <c r="Z15" s="45"/>
-      <c r="AA15" s="45"/>
-      <c r="AB15" s="46"/>
-      <c r="AC15" s="46"/>
-      <c r="AD15" s="47"/>
-      <c r="AE15" s="47"/>
-      <c r="AF15" s="48"/>
-      <c r="AG15" s="48"/>
-      <c r="AH15" s="49"/>
-      <c r="AI15" s="49"/>
-      <c r="AJ15" s="56" t="s">
+      <c r="AK15" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="AK15" s="56" t="s">
+      <c r="AL15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="AL15" s="56" t="s">
+      <c r="AM15" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="AM15" s="57" t="s">
+      <c r="AN15" s="31"/>
+      <c r="AO15" s="25"/>
+      <c r="AP15" s="25"/>
+      <c r="AQ15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR15" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="AN15" s="57"/>
-      <c r="AO15" s="51"/>
-      <c r="AP15" s="51"/>
-      <c r="AQ15" s="52" t="s">
+      <c r="AS15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT15" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU15" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV15" s="32"/>
+      <c r="AW15" s="23"/>
+      <c r="AX15" s="23"/>
+      <c r="AY15" s="27"/>
+      <c r="AZ15" s="27"/>
+      <c r="BA15" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AR15" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS15" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT15" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU15" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV15" s="58"/>
-      <c r="AW15" s="49"/>
-      <c r="AX15" s="49"/>
-      <c r="AY15" s="53"/>
-      <c r="AZ15" s="53"/>
-      <c r="BA15" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="BB15" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC15" s="38"/>
-      <c r="BD15" s="48" t="s">
+      <c r="BC15" s="13"/>
+      <c r="BD15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="BE15" s="48" t="s">
+      <c r="BE15" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="BF15" s="39"/>
+      <c r="BF15" s="14"/>
       <c r="BG15" s="0"/>
       <c r="BH15" s="0"/>
       <c r="BI15" s="0"/>
@@ -15790,142 +15132,142 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="R16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="T16" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="41" t="s">
+      <c r="U16" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="M16" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="N16" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="O16" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="P16" s="55" t="s">
+      <c r="V16" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="W16" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="R16" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="S16" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="T16" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="U16" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="V16" s="43" t="s">
+      <c r="X16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y16" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="W16" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="X16" s="44" t="s">
+      <c r="Z16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA16" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="Y16" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z16" s="45" t="s">
+      <c r="AB16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC16" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="AA16" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB16" s="46" t="s">
+      <c r="AD16" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE16" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="AC16" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD16" s="47" t="s">
+      <c r="AF16" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="AE16" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF16" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG16" s="48"/>
-      <c r="AH16" s="49" t="s">
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="AI16" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ16" s="66"/>
-      <c r="AK16" s="66"/>
-      <c r="AL16" s="66"/>
-      <c r="AM16" s="57" t="s">
+      <c r="AJ16" s="40"/>
+      <c r="AK16" s="40"/>
+      <c r="AL16" s="40"/>
+      <c r="AM16" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN16" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AN16" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO16" s="51" t="s">
+      <c r="AO16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP16" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="AP16" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="AQ16" s="68"/>
-      <c r="AR16" s="68"/>
-      <c r="AS16" s="68"/>
-      <c r="AT16" s="68"/>
-      <c r="AU16" s="58" t="s">
+      <c r="AQ16" s="42"/>
+      <c r="AR16" s="42"/>
+      <c r="AS16" s="42"/>
+      <c r="AT16" s="42"/>
+      <c r="AU16" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AV16" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="AW16" s="49" t="s">
+      <c r="AW16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="AX16" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY16" s="53"/>
-      <c r="AZ16" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="BA16" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="BB16" s="38" t="s">
+      <c r="AY16" s="27"/>
+      <c r="AZ16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="BC16" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="BD16" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE16" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF16" s="39"/>
+      <c r="BA16" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB16" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="BD16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF16" s="14"/>
       <c r="BG16" s="0"/>
       <c r="BH16" s="0"/>
       <c r="BI16" s="0"/>
@@ -16893,171 +16235,171 @@
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" s="83" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="69" t="n">
+    <row r="17" s="57" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="69" t="n">
+      <c r="B17" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69" t="n">
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="H17" s="70" t="n">
+      <c r="H17" s="44" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="69" t="n">
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="M17" s="69"/>
-      <c r="N17" s="71" t="n">
+      <c r="M17" s="43"/>
+      <c r="N17" s="45" t="n">
         <v>6</v>
       </c>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="59" t="n">
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="33" t="n">
         <v>7</v>
       </c>
-      <c r="S17" s="59"/>
-      <c r="T17" s="59"/>
-      <c r="U17" s="59"/>
-      <c r="V17" s="72" t="n">
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="46" t="n">
         <v>8</v>
       </c>
-      <c r="W17" s="72"/>
-      <c r="X17" s="73" t="n">
+      <c r="W17" s="46"/>
+      <c r="X17" s="47" t="n">
         <v>9</v>
       </c>
-      <c r="Y17" s="73"/>
-      <c r="Z17" s="74" t="n">
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="48" t="n">
         <v>10</v>
       </c>
-      <c r="AA17" s="74"/>
-      <c r="AB17" s="75" t="n">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49" t="n">
         <v>11</v>
       </c>
-      <c r="AC17" s="75"/>
-      <c r="AD17" s="76" t="n">
+      <c r="AC17" s="49"/>
+      <c r="AD17" s="50" t="n">
         <v>12</v>
       </c>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="77" t="n">
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="51" t="n">
         <v>13</v>
       </c>
-      <c r="AG17" s="77" t="n">
+      <c r="AG17" s="51" t="n">
         <v>14</v>
       </c>
-      <c r="AH17" s="78" t="n">
+      <c r="AH17" s="52" t="n">
         <v>15</v>
       </c>
-      <c r="AI17" s="78"/>
-      <c r="AJ17" s="79" t="n">
+      <c r="AI17" s="52"/>
+      <c r="AJ17" s="53" t="n">
         <v>16</v>
       </c>
-      <c r="AK17" s="79"/>
-      <c r="AL17" s="79"/>
-      <c r="AM17" s="79"/>
-      <c r="AN17" s="79"/>
-      <c r="AO17" s="80" t="n">
+      <c r="AK17" s="53"/>
+      <c r="AL17" s="53"/>
+      <c r="AM17" s="53"/>
+      <c r="AN17" s="53"/>
+      <c r="AO17" s="54" t="n">
         <v>17</v>
       </c>
-      <c r="AP17" s="80"/>
-      <c r="AQ17" s="81" t="n">
+      <c r="AP17" s="54"/>
+      <c r="AQ17" s="55" t="n">
         <v>18</v>
       </c>
-      <c r="AR17" s="81"/>
-      <c r="AS17" s="81"/>
-      <c r="AT17" s="81"/>
-      <c r="AU17" s="81"/>
-      <c r="AV17" s="81"/>
-      <c r="AW17" s="78" t="n">
+      <c r="AR17" s="55"/>
+      <c r="AS17" s="55"/>
+      <c r="AT17" s="55"/>
+      <c r="AU17" s="55"/>
+      <c r="AV17" s="55"/>
+      <c r="AW17" s="52" t="n">
         <v>19</v>
       </c>
-      <c r="AX17" s="78"/>
-      <c r="AY17" s="78" t="n">
+      <c r="AX17" s="52"/>
+      <c r="AY17" s="52" t="n">
         <v>20</v>
       </c>
-      <c r="AZ17" s="78" t="n">
+      <c r="AZ17" s="52" t="n">
         <v>21</v>
       </c>
-      <c r="BA17" s="59"/>
-      <c r="BB17" s="59" t="n">
+      <c r="BA17" s="33"/>
+      <c r="BB17" s="33" t="n">
         <v>22</v>
       </c>
-      <c r="BC17" s="59"/>
-      <c r="BD17" s="59"/>
-      <c r="BE17" s="59"/>
-      <c r="BF17" s="82" t="n">
+      <c r="BC17" s="33"/>
+      <c r="BD17" s="33"/>
+      <c r="BE17" s="33"/>
+      <c r="BF17" s="56" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="69"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="71"/>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
-      <c r="Q18" s="71"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="72"/>
-      <c r="W18" s="72"/>
-      <c r="X18" s="73"/>
-      <c r="Y18" s="87"/>
-      <c r="Z18" s="74"/>
-      <c r="AA18" s="74"/>
-      <c r="AB18" s="75"/>
-      <c r="AC18" s="75"/>
-      <c r="AD18" s="76"/>
-      <c r="AE18" s="76"/>
-      <c r="AF18" s="59"/>
-      <c r="AG18" s="59"/>
-      <c r="AH18" s="78"/>
-      <c r="AI18" s="78"/>
-      <c r="AJ18" s="79"/>
-      <c r="AK18" s="79"/>
-      <c r="AL18" s="79"/>
-      <c r="AM18" s="79"/>
-      <c r="AN18" s="79"/>
-      <c r="AO18" s="80"/>
-      <c r="AP18" s="80"/>
-      <c r="AQ18" s="81"/>
-      <c r="AR18" s="81"/>
-      <c r="AS18" s="81"/>
-      <c r="AT18" s="81"/>
-      <c r="AU18" s="81"/>
-      <c r="AV18" s="81"/>
-      <c r="AW18" s="78"/>
-      <c r="AX18" s="78"/>
-      <c r="AY18" s="78"/>
-      <c r="AZ18" s="78"/>
-      <c r="BA18" s="59"/>
-      <c r="BB18" s="59"/>
-      <c r="BC18" s="59"/>
-      <c r="BD18" s="59"/>
-      <c r="BE18" s="59"/>
-      <c r="BF18" s="88"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="47"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="48"/>
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="49"/>
+      <c r="AD18" s="50"/>
+      <c r="AE18" s="50"/>
+      <c r="AF18" s="33"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="52"/>
+      <c r="AI18" s="52"/>
+      <c r="AJ18" s="53"/>
+      <c r="AK18" s="53"/>
+      <c r="AL18" s="53"/>
+      <c r="AM18" s="53"/>
+      <c r="AN18" s="53"/>
+      <c r="AO18" s="54"/>
+      <c r="AP18" s="54"/>
+      <c r="AQ18" s="55"/>
+      <c r="AR18" s="55"/>
+      <c r="AS18" s="55"/>
+      <c r="AT18" s="55"/>
+      <c r="AU18" s="55"/>
+      <c r="AV18" s="55"/>
+      <c r="AW18" s="52"/>
+      <c r="AX18" s="52"/>
+      <c r="AY18" s="52"/>
+      <c r="AZ18" s="52"/>
+      <c r="BA18" s="33"/>
+      <c r="BB18" s="33"/>
+      <c r="BC18" s="33"/>
+      <c r="BD18" s="33"/>
+      <c r="BE18" s="33"/>
+      <c r="BF18" s="62"/>
       <c r="BG18" s="0"/>
       <c r="BH18" s="0"/>
       <c r="BI18" s="0"/>
@@ -18025,177 +17367,177 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" s="119" customFormat="true" ht="16.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="89"/>
-      <c r="B19" s="90" t="s">
+    <row r="19" s="94" customFormat="true" ht="16.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="63"/>
+      <c r="B19" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="D19" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="90" t="s">
+      <c r="E19" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="90" t="s">
+      <c r="F19" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="G19" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="91" t="s">
+      <c r="H19" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="92" t="s">
+      <c r="I19" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="93" t="s">
+      <c r="J19" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="94" t="s">
+      <c r="K19" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="K19" s="94" t="s">
+      <c r="L19" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="L19" s="95" t="s">
+      <c r="M19" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="M19" s="91" t="s">
+      <c r="N19" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="N19" s="96" t="s">
+      <c r="O19" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="O19" s="96" t="s">
+      <c r="P19" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="P19" s="97" t="s">
+      <c r="Q19" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="Q19" s="97" t="s">
+      <c r="R19" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="R19" s="98" t="s">
+      <c r="S19" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="S19" s="98" t="s">
+      <c r="T19" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="T19" s="98" t="s">
+      <c r="U19" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="U19" s="99" t="s">
-        <v>70</v>
-      </c>
-      <c r="V19" s="100" t="s">
+      <c r="V19" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="W19" s="100" t="s">
+      <c r="W19" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="X19" s="101" t="s">
+      <c r="X19" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="Y19" s="102" t="s">
+      <c r="Y19" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="Z19" s="103" t="s">
+      <c r="Z19" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="AA19" s="104" t="s">
+      <c r="AA19" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="AB19" s="105" t="s">
+      <c r="AB19" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="AC19" s="106" t="s">
+      <c r="AC19" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="AD19" s="107" t="s">
+      <c r="AD19" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="AE19" s="108" t="s">
+      <c r="AE19" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="AF19" s="109" t="s">
+      <c r="AF19" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="AG19" s="110" t="s">
+      <c r="AG19" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="AH19" s="111" t="s">
+      <c r="AH19" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="AI19" s="112" t="s">
+      <c r="AI19" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="AJ19" s="113" t="s">
+      <c r="AJ19" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="AK19" s="113" t="s">
+      <c r="AK19" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="AL19" s="113" t="s">
+      <c r="AL19" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="AM19" s="114" t="s">
+      <c r="AM19" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="AN19" s="113" t="s">
+      <c r="AN19" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="AO19" s="115" t="s">
+      <c r="AO19" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="AP19" s="116" t="s">
+      <c r="AP19" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="AQ19" s="117" t="s">
+      <c r="AQ19" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="AR19" s="117" t="s">
+      <c r="AR19" s="91" t="s">
         <v>99</v>
       </c>
-      <c r="AS19" s="117" t="s">
+      <c r="AS19" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="AT19" s="117" t="s">
+      <c r="AT19" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="AU19" s="118" t="s">
+      <c r="AU19" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="AV19" s="117" t="s">
+      <c r="AV19" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="AW19" s="111" t="s">
+      <c r="AW19" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AX19" s="112" t="s">
+      <c r="AX19" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="AY19" s="112" t="s">
+      <c r="AY19" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="AZ19" s="112" t="s">
+      <c r="AZ19" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="BA19" s="98" t="s">
+      <c r="BA19" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="BB19" s="98" t="s">
+      <c r="BB19" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="BC19" s="99" t="s">
+      <c r="BC19" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="BD19" s="99" t="s">
+      <c r="BD19" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="BE19" s="99" t="s">
+      <c r="BE19" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="BF19" s="91" t="s">
+      <c r="BF19" s="93" t="s">
         <v>113</v>
       </c>
     </row>
@@ -18204,8 +17546,8 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B13:F16"/>

</xml_diff>